<commit_message>
I have added the notebook
</commit_message>
<xml_diff>
--- a/notebooks/validation_data.xlsx
+++ b/notebooks/validation_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,431 +496,390 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>43450.1875</v>
+        <v>44370.10416666666</v>
       </c>
       <c r="B2" t="n">
-        <v>1771088</v>
+        <v>1769019</v>
       </c>
       <c r="C2" t="n">
-        <v>26834047</v>
+        <v>129718949</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>../recordings/2018/12/16/recordings_1771088_26834047_20181216_043000.wav</t>
+          <t>../recordings/2021/06/23/recordings_1769019_129718949_20210623_023000.wav</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>E16</t>
+          <t>E7</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ZWOODF110</t>
+          <t>ZWOODF39</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Boundary Box</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Unstructured audio files/2018/12/16/recordings_1771088_26834047_20181216_043000.wav</t>
+          <t>Unstructured audio files/2021/06/23/recordings_1769019_129718949_20210623_023000.wav</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>43450.1875</v>
+        <v>43965.15625</v>
       </c>
       <c r="B3" t="n">
-        <v>1628286</v>
+        <v>7017095</v>
       </c>
       <c r="C3" t="n">
-        <v>26947832</v>
+        <v>74345861</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>../recordings/2018/12/16/recordings_1628286_26947832_20181216_043000.wav</t>
+          <t>../recordings/2020/05/14/recordings_7017095_74345861_20200514_034500.wav</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>GU2</t>
+          <t>CR0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ZPEWLY04</t>
+          <t>ZRUSSH10</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Service Pipe</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Unstructured audio files/2018/12/16/recordings_1628286_26947832_20181216_043000.wav</t>
+          <t>Unstructured audio files/2020/05/14/recordings_7017095_74345861_20200514_034500.wav</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>43450.1875</v>
+        <v>43980.15625</v>
       </c>
       <c r="B4" t="n">
-        <v>1657491</v>
+        <v>1613699</v>
       </c>
       <c r="C4" t="n">
-        <v>26877815</v>
+        <v>76414165</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>../recordings/2018/12/16/recordings_1657491_26877815_20181216_043000.wav</t>
+          <t>../recordings/2020/05/29/recordings_1613699_76414165_20200529_034500.wav</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>SL7</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ZEALNG25</t>
+          <t>ZMARLT03</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I4" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Boundary Box</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Unstructured audio files/2018/12/16/recordings_1657491_26877815_20181216_043000.wav</t>
+          <t>Unstructured audio files/2020/05/29/recordings_1613699_76414165_20200529_034500.wav</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>43450.1875</v>
+        <v>44455.10416666666</v>
       </c>
       <c r="B5" t="n">
-        <v>1720029</v>
+        <v>1722290</v>
       </c>
       <c r="C5" t="n">
-        <v>26889767</v>
+        <v>143471783</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>../recordings/2018/12/16/recordings_1720029_26889767_20181216_043000.wav</t>
+          <t>../recordings/2021/09/16/recordings_1722290_143471783_20210916_023000.wav</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WC1X</t>
+          <t>E14</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ZMAIDL59</t>
+          <t>ZFINSB56</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
+        <v>25</v>
+      </c>
+      <c r="I5" t="n">
         <v>5</v>
       </c>
-      <c r="I5" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Main</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Unstructured audio files/2018/12/16/recordings_1720029_26889767_20181216_043000.wav</t>
+          <t>Unstructured audio files/2021/09/16/recordings_1722290_143471783_20210916_023000.wav</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>43446.16666666666</v>
+        <v>44198.15625</v>
       </c>
       <c r="B6" t="n">
-        <v>1740155</v>
+        <v>1771081</v>
       </c>
       <c r="C6" t="n">
-        <v>26586796</v>
+        <v>104929501</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>../recordings/2018/12/12/recordings_1740155_26586796_20181212_040000.wav</t>
+          <t>../recordings/2021/01/02/recordings_1771081_104929501_20210102_034500.wav</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>E17</t>
+          <t>E7</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ZWOODF93</t>
+          <t>ZWOODF39</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="I6" t="n">
-        <v>4</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Service Pipe</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Unstructured audio files/2018/12/12/recordings_1740155_26586796_20181212_040000.wav</t>
+          <t>Unstructured audio files/2021/01/02/recordings_1771081_104929501_20210102_034500.wav</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44370.10416666666</v>
+        <v>43450.1875</v>
       </c>
       <c r="B7" t="n">
-        <v>1769019</v>
+        <v>1628286</v>
       </c>
       <c r="C7" t="n">
-        <v>129718949</v>
+        <v>26947832</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>../recordings/2021/06/23/recordings_1769019_129718949_20210623_023000.wav</t>
+          <t>../recordings/2018/12/16/recordings_1628286_26947832_20181216_043000.wav</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>E7</t>
+          <t>GU2</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ZWOODF39</t>
+          <t>ZPEWLY04</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="I7" t="n">
-        <v>10</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Boundary Box</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Unstructured audio files/2021/06/23/recordings_1769019_129718949_20210623_023000.wav</t>
+          <t>Unstructured audio files/2018/12/16/recordings_1628286_26947832_20181216_043000.wav</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>43965.15625</v>
+        <v>43450.1875</v>
       </c>
       <c r="B8" t="n">
-        <v>7017095</v>
+        <v>1657491</v>
       </c>
       <c r="C8" t="n">
-        <v>74345861</v>
+        <v>26877815</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>../recordings/2020/05/14/recordings_7017095_74345861_20200514_034500.wav</t>
+          <t>../recordings/2018/12/16/recordings_1657491_26877815_20181216_043000.wav</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CR0</t>
+          <t>W3</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ZRUSSH10</t>
+          <t>ZEALNG25</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="I8" t="n">
-        <v>7</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Service Pipe</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Unstructured audio files/2020/05/14/recordings_7017095_74345861_20200514_034500.wav</t>
+          <t>Unstructured audio files/2018/12/16/recordings_1657491_26877815_20181216_043000.wav</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>43980.15625</v>
+        <v>43450.1875</v>
       </c>
       <c r="B9" t="n">
-        <v>1613699</v>
+        <v>1720029</v>
       </c>
       <c r="C9" t="n">
-        <v>76414165</v>
+        <v>26889767</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>../recordings/2020/05/29/recordings_1613699_76414165_20200529_034500.wav</t>
+          <t>../recordings/2018/12/16/recordings_1720029_26889767_20181216_043000.wav</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>SL7</t>
+          <t>WC1X</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>ZMARLT03</t>
+          <t>ZMAIDL59</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I9" t="n">
-        <v>5</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Boundary Box</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Unstructured audio files/2020/05/29/recordings_1613699_76414165_20200529_034500.wav</t>
+          <t>Unstructured audio files/2018/12/16/recordings_1720029_26889767_20181216_043000.wav</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44455.10416666666</v>
+        <v>43446.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>1722290</v>
+        <v>1740155</v>
       </c>
       <c r="C10" t="n">
-        <v>143471783</v>
+        <v>26586796</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>../recordings/2021/09/16/recordings_1722290_143471783_20210916_023000.wav</t>
+          <t>../recordings/2018/12/12/recordings_1740155_26586796_20181212_040000.wav</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>E14</t>
+          <t>E17</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>ZFINSB56</t>
+          <t>ZWOODF93</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="I10" t="n">
-        <v>5</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Main</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Unstructured audio files/2021/09/16/recordings_1722290_143471783_20210916_023000.wav</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>44198.15625</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1771081</v>
-      </c>
-      <c r="C11" t="n">
-        <v>104929501</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>../recordings/2021/01/02/recordings_1771081_104929501_20210102_034500.wav</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>E7</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>ZWOODF39</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" t="n">
-        <v>24</v>
-      </c>
-      <c r="I11" t="n">
-        <v>7</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Service Pipe</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Unstructured audio files/2021/01/02/recordings_1771081_104929501_20210102_034500.wav</t>
+          <t>Unstructured audio files/2018/12/12/recordings_1740155_26586796_20181212_040000.wav</t>
         </is>
       </c>
     </row>

</xml_diff>